<commit_message>
Ispravka u kodu i fajlu za analizu anotacije.
</commit_message>
<xml_diff>
--- a/pythonProject/tokenized_files/summary.xlsx
+++ b/pythonProject/tokenized_files/summary.xlsx
@@ -537,10 +537,10 @@
         <v>269</v>
       </c>
       <c r="L2" t="n">
-        <v>840</v>
+        <v>1215</v>
       </c>
       <c r="M2" t="n">
-        <v>4807</v>
+        <v>5182</v>
       </c>
     </row>
     <row r="3">
@@ -580,10 +580,10 @@
         <v>269</v>
       </c>
       <c r="L3" t="n">
-        <v>1099</v>
+        <v>982</v>
       </c>
       <c r="M3" t="n">
-        <v>5259</v>
+        <v>5142</v>
       </c>
     </row>
     <row r="4">
@@ -623,10 +623,10 @@
         <v>143</v>
       </c>
       <c r="L4" t="n">
-        <v>777</v>
+        <v>408</v>
       </c>
       <c r="M4" t="n">
-        <v>5447</v>
+        <v>5078</v>
       </c>
     </row>
     <row r="5">
@@ -666,10 +666,10 @@
         <v>7</v>
       </c>
       <c r="L5" t="n">
-        <v>49</v>
+        <v>150</v>
       </c>
       <c r="M5" t="n">
-        <v>4905</v>
+        <v>5006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>